<commit_message>
added different deployment options
</commit_message>
<xml_diff>
--- a/LBD Deployment Helper - 5 Node.xlsx
+++ b/LBD Deployment Helper - 5 Node.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nclouse\Google Drive\Personal\blog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan.Clouse\OneDrive - mcaConnect, LLC\Personal\Github\LBD Helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214A0A41-9474-4E48-AE6A-47ED55DFCC9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{214A0A41-9474-4E48-AE6A-47ED55DFCC9C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{BCC63253-1D14-402B-8199-F498CFA43597}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="5" r:id="rId1"/>
     <sheet name="Copy To Nodes" sheetId="6" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="70">
   <si>
     <t>DNS Name</t>
   </si>
@@ -174,9 +175,6 @@
     <t>AXDBAdmin</t>
   </si>
   <si>
-    <t>Account</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -217,6 +215,33 @@
   </si>
   <si>
     <t>Copy InfrastructureScripts To ADFS From Share</t>
+  </si>
+  <si>
+    <t>Account Name</t>
+  </si>
+  <si>
+    <t>Domain Account</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>4 character code for this environment. Examples are DEMO, TEST, MIG, GOLD.</t>
+  </si>
+  <si>
+    <t>UNC for root file share for this environment where aos-storage and agent folders will go</t>
+  </si>
+  <si>
+    <t>root domain name unqualitified. If your domain is new.contoso.com, contoso.com, sub.new.contoso.com, use value "contoso"</t>
+  </si>
+  <si>
+    <t>The preferred DNS zone for this cluster</t>
+  </si>
+  <si>
+    <t>Where the Infrastructre scripts will be shared</t>
+  </si>
+  <si>
+    <t>Where the Infrastructre scripts for VMs will be shared</t>
   </si>
 </sst>
 </file>
@@ -295,7 +320,11 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -309,8 +338,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E6545BA-ED1A-419A-A665-DA8CB4E439DA}" name="Table1" displayName="Table1" ref="A1:D10" totalsRowShown="0">
-  <autoFilter ref="A1:D10" xr:uid="{5652AF24-9672-4D72-AE8D-38DB15A8C2DB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E6545BA-ED1A-419A-A665-DA8CB4E439DA}" name="Table1" displayName="Table1" ref="A2:D11" totalsRowShown="0">
+  <autoFilter ref="A2:D11" xr:uid="{5652AF24-9672-4D72-AE8D-38DB15A8C2DB}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D08047A9-54B2-45D2-8683-B005348AE464}" name="Machine Purpose"/>
     <tableColumn id="2" xr3:uid="{6515C1AF-3607-439C-B57E-CC5DD9D60F5F}" name="DNS Name"/>
@@ -322,12 +351,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DB3A15F9-075E-4B5F-9DB2-925FCAA04ECF}" name="Table3" displayName="Table3" ref="A12:C19" totalsRowShown="0">
-  <autoFilter ref="A12:C19" xr:uid="{4A5EB2B6-A25A-4372-A0E8-AA6F9AF94FCC}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{B243BC49-71C0-46BC-9631-68240D16A6A9}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{DCFE744D-3622-429E-A30A-05B766944BD6}" name="Account"/>
-    <tableColumn id="3" xr3:uid="{E0928889-BAF9-4EDA-BFA9-793FDC6D2D4F}" name="Type"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ED803CF8-9C30-4D5E-8B28-5012490D5F09}" name="Table33" displayName="Table33" ref="A13:D20" totalsRowShown="0">
+  <autoFilter ref="A13:D20" xr:uid="{8B8EE426-08C9-445A-A784-43F00E7A2F79}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{ECFB918C-EC90-4A8A-9AFA-3B2FE2271C9F}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{8E5059B6-BBE1-4A0F-B1C6-AABAE14935FD}" name="Account Name" dataDxfId="0">
+      <calculatedColumnFormula>LEFT(A14,4) &amp; $G$2 &amp; MID(A14,5,10)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{7FD9AC2E-607D-46A4-8D0E-270AE27C208F}" name="Domain Account"/>
+    <tableColumn id="4" xr3:uid="{3859AE27-90BD-4940-9FC7-187AEE0DB954}" name="Type"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{ECD483CA-9246-4DA9-9558-0279F79CD57A}" name="Table2" displayName="Table2" ref="H1:H9" totalsRowShown="0">
+  <autoFilter ref="H1:H9" xr:uid="{989589CD-1A51-4D31-8DF2-68A4E642923A}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{2C0AC706-E31B-4EF9-945F-550D2F77C4A3}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -630,320 +672,375 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A87E3A0-AE97-4BFF-831F-BBF3B46CBBC6}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.7109375" customWidth="1"/>
-    <col min="7" max="7" width="47" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="116" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="H2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="2" t="str">
-        <f>"\\" &amp; B4 &amp; "\D365\" &amp; G1</f>
-        <v>\\AAX-PFS-01\D365\TEST</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="G3" s="2" t="str">
+        <f>"\\" &amp; B5 &amp; "\D365\" &amp; G2</f>
+        <v>\\AAX-PFS-01\D365\TEST</v>
+      </c>
+      <c r="H3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>
       <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="2" t="str">
-        <f>"ax" &amp; G1 &amp; "."&amp;G4&amp;"."&amp;G3&amp;".com"</f>
+      <c r="G6" s="2" t="str">
+        <f>"ax" &amp; G2 &amp; "."&amp;G5&amp;"."&amp;G4&amp;".com"</f>
         <v>axTEST.d365ffo.onprem.atomicax.com</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="2" t="str">
-        <f>"sf" &amp; G1 &amp;"."&amp;G4&amp;"."&amp;G3&amp;".com"</f>
+      <c r="G7" s="2" t="str">
+        <f>"sf" &amp; G2 &amp;"."&amp;G5&amp;"."&amp;G4&amp;".com"</f>
         <v>sfTEST.d365ffo.onprem.atomicax.com</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="2" t="str">
-        <f>G2&amp;"\InfrastructureScripts"</f>
-        <v>\\AAX-PFS-01\D365\TEST\InfrastructureScripts</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
       </c>
       <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="2" t="str">
+        <f>G3&amp;"\InfrastructureScripts"</f>
+        <v>\\AAX-PFS-01\D365\TEST\InfrastructureScripts</v>
+      </c>
+      <c r="H8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="2" t="str">
-        <f>G7 &amp; "VMs"</f>
+      <c r="G9" s="2" t="str">
+        <f>G8 &amp; "VMs"</f>
         <v>\\AAX-PFS-01\D365\TEST\InfrastructureScriptsVMs</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="H9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" t="s">
         <v>47</v>
       </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B14" t="str">
+        <f t="shared" ref="B14:B20" si="0">LEFT(A14,4) &amp; $G$2 &amp; MID(A14,5,10)</f>
+        <v>svc-TESTFRAS$</v>
+      </c>
+      <c r="C14" t="str">
+        <f>$G$4 &amp; "\" &amp; LEFT(A14,4) &amp; $G$2 &amp; MID(A14,5,10)</f>
+        <v>atomicax\svc-TESTFRAS$</v>
+      </c>
+      <c r="D14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>49</v>
       </c>
-      <c r="B13" t="str">
-        <f>$G$3 &amp; "\" &amp; LEFT(A13,4) &amp; $G$1 &amp; MID(A13,5,10)</f>
-        <v>atomicax\svc-TESTFRAS$</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>svc-TESTFRPS$</v>
+      </c>
+      <c r="C15" t="str">
+        <f>$G$4 &amp; "\" &amp; LEFT(A15,4) &amp; $G$2 &amp; MID(A15,5,10)</f>
+        <v>atomicax\svc-TESTFRPS$</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>svc-TESTFRCO$</v>
+      </c>
+      <c r="C16" t="str">
+        <f>$G$4 &amp; "\" &amp; LEFT(A16,4) &amp; $G$2 &amp; MID(A16,5,10)</f>
+        <v>atomicax\svc-TESTFRCO$</v>
+      </c>
+      <c r="D16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>svc-TESTAXSF$</v>
+      </c>
+      <c r="C17" t="str">
+        <f>$G$4 &amp; "\" &amp; LEFT(A17,4) &amp; $G$2 &amp; MID(A17,5,10)</f>
+        <v>atomicax\svc-TESTAXSF$</v>
+      </c>
+      <c r="D17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="str">
+        <f>LEFT(A18,2) &amp; $G$2 &amp; MID(A18,3,100)</f>
+        <v>AXTESTServiceUser</v>
+      </c>
+      <c r="C18" t="str">
+        <f>G4&amp; "\" &amp; LEFT(A18,2) &amp; G2 &amp; MID(A18,3,20)</f>
+        <v>atomicax\AXTESTServiceUser</v>
+      </c>
+      <c r="D18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" t="str">
-        <f>$G$3 &amp; "\" &amp; LEFT(A14,4) &amp; $G$1 &amp; MID(A14,5,10)</f>
-        <v>atomicax\svc-TESTFRPS$</v>
-      </c>
-      <c r="C14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" t="str">
-        <f>$G$3 &amp; "\" &amp; LEFT(A15,4) &amp; $G$1 &amp; MID(A15,5,10)</f>
-        <v>atomicax\svc-TESTFRCO$</v>
-      </c>
-      <c r="C15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" t="str">
-        <f>$G$3 &amp; "\" &amp; LEFT(A16,4) &amp; $G$1 &amp; MID(A16,5,10)</f>
-        <v>atomicax\svc-TESTAXSF$</v>
-      </c>
-      <c r="C16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>AXDBTESTAdmin</v>
+      </c>
+      <c r="C19" t="str">
+        <f xml:space="preserve"> LEFT(A19,4) &amp; $G$2 &amp; MID(A19,5,10)</f>
+        <v>AXDBTESTAdmin</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>53</v>
       </c>
-      <c r="B17" t="str">
-        <f>G3 &amp; "\" &amp; LEFT(A17,2) &amp; G1 &amp; MID(A17,3,20)</f>
-        <v>atomicax\AXTESTServiceUser</v>
-      </c>
-      <c r="C17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" t="str">
-        <f>A18</f>
-        <v>AXDBAdmin</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>Svc-TESTLA$</v>
+      </c>
+      <c r="C20" t="str">
+        <f>$G$4 &amp; "\" &amp; LEFT(A20,4) &amp; $G$2 &amp; MID(A20,5,10)</f>
+        <v>atomicax\Svc-TESTLA$</v>
+      </c>
+      <c r="D20" t="s">
         <v>54</v>
-      </c>
-      <c r="B19" t="str">
-        <f>$G$3 &amp; "\" &amp; LEFT(A19,4) &amp; $G$1 &amp; MID(A19,5,10)</f>
-        <v>atomicax\Svc-TESTLA$</v>
-      </c>
-      <c r="C19" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="\\AAX-PFS-01\d365\TEST" xr:uid="{DF2E5AED-1C02-4998-BDEC-B0C17DD670CA}"/>
+    <hyperlink ref="G3" r:id="rId1" display="\\AAX-PFS-01\d365\TEST" xr:uid="{DF2E5AED-1C02-4998-BDEC-B0C17DD670CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -953,7 +1050,7 @@
   <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="A8" sqref="A8:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,99 +1060,99 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f>"robocopy " &amp; Setup!$G$2 &amp; "\InfrastructureScripts \\" &amp; Setup!B6 &amp; "\c$\InfrastructureScripts /mir"</f>
+        <f>"robocopy " &amp; Setup!$G$3 &amp; "\InfrastructureScripts \\" &amp; Setup!B7 &amp; "\c$\InfrastructureScripts /mir"</f>
         <v>robocopy \\AAX-PFS-01\D365\TEST\InfrastructureScripts \\AAX-TAOS-01\c$\InfrastructureScripts /mir</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f>"robocopy " &amp; Setup!$G$2 &amp; "\InfrastructureScripts \\" &amp; Setup!B7 &amp; "\c$\InfrastructureScripts /mir"</f>
+        <f>"robocopy " &amp; Setup!$G$3 &amp; "\InfrastructureScripts \\" &amp; Setup!B8 &amp; "\c$\InfrastructureScripts /mir"</f>
         <v>robocopy \\AAX-PFS-01\D365\TEST\InfrastructureScripts \\AAX-TORCH-01\c$\InfrastructureScripts /mir</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f>"robocopy " &amp; Setup!$G$2 &amp; "\InfrastructureScripts \\" &amp; Setup!B8 &amp; "\c$\InfrastructureScripts /mir"</f>
+        <f>"robocopy " &amp; Setup!$G$3 &amp; "\InfrastructureScripts \\" &amp; Setup!B9 &amp; "\c$\InfrastructureScripts /mir"</f>
         <v>robocopy \\AAX-PFS-01\D365\TEST\InfrastructureScripts \\AAX-TORCH-02\c$\InfrastructureScripts /mir</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
-        <f>"robocopy " &amp; Setup!$G$2 &amp; "\InfrastructureScripts \\" &amp; Setup!B9 &amp; "\c$\InfrastructureScripts /mir"</f>
+        <f>"robocopy " &amp; Setup!$G$3 &amp; "\InfrastructureScripts \\" &amp; Setup!B10 &amp; "\c$\InfrastructureScripts /mir"</f>
         <v>robocopy \\AAX-PFS-01\D365\TEST\InfrastructureScripts \\AAX-TMR-01\c$\InfrastructureScripts /mir</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f>"robocopy " &amp; Setup!$G$2 &amp; "\InfrastructureScripts \\" &amp; Setup!B10 &amp; "\c$\InfrastructureScripts /mir"</f>
+        <f>"robocopy " &amp; Setup!$G$3 &amp; "\InfrastructureScripts \\" &amp; Setup!B11 &amp; "\c$\InfrastructureScripts /mir"</f>
         <v>robocopy \\AAX-PFS-01\D365\TEST\InfrastructureScripts \\AAX-TSSRS-01\c$\InfrastructureScripts /mir</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f>"robocopy " &amp; Setup!$G$2 &amp; "\InfrastructureScripts \\" &amp; Setup!B11 &amp; "\c$\InfrastructureScripts /mir"</f>
+        <f>"robocopy " &amp; Setup!$G$3 &amp; "\InfrastructureScripts \\" &amp; Setup!B12 &amp; "\c$\InfrastructureScripts /mir"</f>
         <v>robocopy \\AAX-PFS-01\D365\TEST\InfrastructureScripts \\\c$\InfrastructureScripts /mir</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f>"robocopy  c:\InfrastructureScripts " &amp; Setup!$G$2 &amp; "\InfrastructureScripts /mir"</f>
+        <f>"robocopy  c:\InfrastructureScripts " &amp; Setup!$G$3 &amp; "\InfrastructureScripts /mir"</f>
         <v>robocopy  c:\InfrastructureScripts \\AAX-PFS-01\D365\TEST\InfrastructureScripts /mir</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f>"robocopy " &amp; Setup!$G$2 &amp;"\InfrastructureScripts\VMs\" &amp; Setup!B6 &amp; " \\" &amp; Setup!B6 &amp; "\c$\InfrasctureScriptsVMs\ /MIR"</f>
+        <f>"robocopy " &amp; Setup!$G$3 &amp;"\InfrastructureScripts\VMs\" &amp; Setup!B7 &amp; " \\" &amp; Setup!B7 &amp; "\c$\InfrasctureScriptsVMs\ /MIR"</f>
         <v>robocopy \\AAX-PFS-01\D365\TEST\InfrastructureScripts\VMs\AAX-TAOS-01 \\AAX-TAOS-01\c$\InfrasctureScriptsVMs\ /MIR</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f>"robocopy " &amp; Setup!$G$2 &amp;"\InfrastructureScripts\VMs\" &amp; Setup!B7 &amp; " \\" &amp; Setup!B7 &amp; "\c$\InfrasctureScriptsVMs\ /MIR"</f>
+        <f>"robocopy " &amp; Setup!$G$3 &amp;"\InfrastructureScripts\VMs\" &amp; Setup!B8 &amp; " \\" &amp; Setup!B8 &amp; "\c$\InfrasctureScriptsVMs\ /MIR"</f>
         <v>robocopy \\AAX-PFS-01\D365\TEST\InfrastructureScripts\VMs\AAX-TORCH-01 \\AAX-TORCH-01\c$\InfrasctureScriptsVMs\ /MIR</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>"robocopy " &amp; Setup!$G$2 &amp;"\InfrastructureScripts\VMs\" &amp; Setup!B8 &amp; " \\" &amp; Setup!B8 &amp; "\c$\InfrasctureScriptsVMs\ /MIR"</f>
+        <f>"robocopy " &amp; Setup!$G$3 &amp;"\InfrastructureScripts\VMs\" &amp; Setup!B9 &amp; " \\" &amp; Setup!B9 &amp; "\c$\InfrasctureScriptsVMs\ /MIR"</f>
         <v>robocopy \\AAX-PFS-01\D365\TEST\InfrastructureScripts\VMs\AAX-TORCH-02 \\AAX-TORCH-02\c$\InfrasctureScriptsVMs\ /MIR</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f>"robocopy " &amp; Setup!$G$2 &amp;"\InfrastructureScripts\VMs\" &amp; Setup!B9 &amp; " \\" &amp; Setup!B9 &amp; "\c$\InfrasctureScriptsVMs\ /MIR"</f>
+        <f>"robocopy " &amp; Setup!$G$3 &amp;"\InfrastructureScripts\VMs\" &amp; Setup!B10 &amp; " \\" &amp; Setup!B10 &amp; "\c$\InfrasctureScriptsVMs\ /MIR"</f>
         <v>robocopy \\AAX-PFS-01\D365\TEST\InfrastructureScripts\VMs\AAX-TMR-01 \\AAX-TMR-01\c$\InfrasctureScriptsVMs\ /MIR</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f>"robocopy " &amp; Setup!$G$2 &amp;"\InfrastructureScripts\VMs\" &amp; Setup!B10 &amp; " \\" &amp; Setup!B10 &amp; "\c$\InfrasctureScriptsVMs\ /MIR"</f>
+        <f>"robocopy " &amp; Setup!$G$3 &amp;"\InfrastructureScripts\VMs\" &amp; Setup!B11 &amp; " \\" &amp; Setup!B11 &amp; "\c$\InfrasctureScriptsVMs\ /MIR"</f>
         <v>robocopy \\AAX-PFS-01\D365\TEST\InfrastructureScripts\VMs\AAX-TSSRS-01 \\AAX-TSSRS-01\c$\InfrasctureScriptsVMs\ /MIR</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f>"robocopy "&amp;Setup!$G$2&amp;"\InfrastructureScripts \\" &amp; Setup!B4 &amp; "\C$\InfrastructureScripts"</f>
+        <f>"robocopy "&amp;Setup!$G$3&amp;"\InfrastructureScripts \\" &amp; Setup!B5 &amp; "\C$\InfrastructureScripts"</f>
         <v>robocopy \\AAX-PFS-01\D365\TEST\InfrastructureScripts \\AAX-PFS-01\C$\InfrastructureScripts</v>
       </c>
     </row>

</xml_diff>